<commit_message>
Aurrekontua eta laburpena eguneratu
</commit_message>
<xml_diff>
--- a/Proiektua/Aurrekontua/Aurrekontua.xlsx
+++ b/Proiektua/Aurrekontua/Aurrekontua.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julet\GitHub\ProMeta\Proiektua\Aurrekontua\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADF7509-A6E8-4F08-BCF8-FA1F83BD532F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2B1284-7E45-4DB1-9AFF-993C07C3D6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Garatzailea</t>
   </si>
   <si>
-    <t>Testera</t>
-  </si>
-  <si>
     <t>Erremintak</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>Pantheon</t>
+  </si>
+  <si>
+    <t>Probatzailea</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +695,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -730,14 +730,14 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -747,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
@@ -769,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
@@ -792,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4">
         <v>0</v>
@@ -880,7 +880,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -902,7 +902,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -924,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4">
         <v>0</v>
@@ -946,7 +946,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -981,7 +981,7 @@
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>

</xml_diff>